<commit_message>
up to date analysis
</commit_message>
<xml_diff>
--- a/lesion_analysis.xlsx
+++ b/lesion_analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="940" windowWidth="27760" windowHeight="14980" tabRatio="500"/>
+    <workbookView xWindow="-2360" yWindow="460" windowWidth="27760" windowHeight="14980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
   <si>
     <t>blank_eye</t>
   </si>
@@ -85,6 +85,18 @@
   <si>
     <t>wallet_eye_100000</t>
   </si>
+  <si>
+    <t>wallet_eye_000001_2</t>
+  </si>
+  <si>
+    <t>wallet_eye_100001</t>
+  </si>
+  <si>
+    <t>wallet_eye_100000_2</t>
+  </si>
+  <si>
+    <t>wallet_eye_100001_2</t>
+  </si>
 </sst>
 </file>
 
@@ -132,13 +144,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1928,129 +1941,129 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$3:$Q$42</c:f>
+              <c:f>Sheet1!$W$3:$W$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>0.325581</c:v>
+                  <c:v>0.497317</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.370304</c:v>
+                  <c:v>0.593918</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.386404</c:v>
+                  <c:v>0.601073</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.481216</c:v>
+                  <c:v>0.610018</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.533095</c:v>
+                  <c:v>0.627907</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.518784</c:v>
+                  <c:v>0.579606</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.522361</c:v>
+                  <c:v>0.583184</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.527728</c:v>
+                  <c:v>0.617174</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.593918</c:v>
+                  <c:v>0.669052</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.667263</c:v>
+                  <c:v>0.677996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.683363</c:v>
+                  <c:v>0.665474</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.683363</c:v>
+                  <c:v>0.652952</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.683363</c:v>
+                  <c:v>0.677996</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.708408</c:v>
+                  <c:v>0.697674</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.726297</c:v>
+                  <c:v>0.692308</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.733453</c:v>
+                  <c:v>0.677996</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.697674</c:v>
+                  <c:v>0.706619</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.697674</c:v>
+                  <c:v>0.717352</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>0.685152</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.68873</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.694097</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.731664</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.742397</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.738819</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.731664</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.742397</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.754919</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.745975</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.754919</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.779964</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.772809</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.774597</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.769231</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>0.744186</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.763864</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.77102</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.767442</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.769231</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.778175</c:v>
-                </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="34">
+                  <c:v>0.78712</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.78712</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.799642</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>0.774597</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="38">
+                  <c:v>0.774597</c:v>
+                </c:pt>
+                <c:pt idx="39">
                   <c:v>0.788909</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.794275</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.781753</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.785331</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.790698</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.80322</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.80322</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.812165</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.808587</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.810376</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.821109</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.828265</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.831843</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.833631</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.833631</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6243,16 +6256,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>309033</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>64911</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>156633</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>141111</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>156633</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>108655</xdr:rowOff>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>4233</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>184855</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6273,16 +6286,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>444498</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>21167</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>88898</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>46567</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>380999</xdr:colOff>
-      <xdr:row>101</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>25399</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6567,10 +6580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U93"/>
+  <dimension ref="A1:AC93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="AS26" sqref="AS26"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="R51" sqref="R51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6578,7 +6591,7 @@
     <col min="18" max="18" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6619,8 +6632,23 @@
         <v>19</v>
       </c>
       <c r="U1" s="1"/>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" s="1"/>
+      <c r="AB1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -6684,8 +6712,32 @@
       <c r="U2" t="s">
         <v>4</v>
       </c>
+      <c r="V2" t="s">
+        <v>3</v>
+      </c>
+      <c r="W2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>250</v>
       </c>
@@ -6749,8 +6801,32 @@
       <c r="U3">
         <v>0.63506300000000004</v>
       </c>
+      <c r="V3">
+        <v>150302</v>
+      </c>
+      <c r="W3">
+        <v>0.49731700000000001</v>
+      </c>
+      <c r="X3">
+        <v>119736</v>
+      </c>
+      <c r="Y3">
+        <v>0.50268299999999999</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>63737.9</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>0.44901600000000003</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>59677.5</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>0.58855100000000005</v>
+      </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>500</v>
       </c>
@@ -6814,8 +6890,32 @@
       <c r="U4">
         <v>0.63148499999999996</v>
       </c>
+      <c r="V4">
+        <v>41217.1</v>
+      </c>
+      <c r="W4">
+        <v>0.59391799999999995</v>
+      </c>
+      <c r="X4">
+        <v>27230.6</v>
+      </c>
+      <c r="Y4">
+        <v>0.66547400000000001</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>55943.1</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>0.47585</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>43851.5</v>
+      </c>
+      <c r="AC4" s="2">
+        <v>0.62790699999999999</v>
+      </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>750</v>
       </c>
@@ -6879,8 +6979,32 @@
       <c r="U5">
         <v>0.66189600000000004</v>
       </c>
+      <c r="V5">
+        <v>48391.199999999997</v>
+      </c>
+      <c r="W5">
+        <v>0.60107299999999997</v>
+      </c>
+      <c r="X5">
+        <v>30547.1</v>
+      </c>
+      <c r="Y5">
+        <v>0.63863999999999999</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>56902.2</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>0.52593900000000005</v>
+      </c>
+      <c r="AB5" s="2">
+        <v>37687.599999999999</v>
+      </c>
+      <c r="AC5" s="2">
+        <v>0.660107</v>
+      </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1000</v>
       </c>
@@ -6944,8 +7068,32 @@
       <c r="U6">
         <v>0.68157400000000001</v>
       </c>
+      <c r="V6">
+        <v>41375.9</v>
+      </c>
+      <c r="W6">
+        <v>0.61001799999999995</v>
+      </c>
+      <c r="X6">
+        <v>24490</v>
+      </c>
+      <c r="Y6">
+        <v>0.70482999999999996</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>36569.199999999997</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>0.56529499999999999</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>48125.599999999999</v>
+      </c>
+      <c r="AC6" s="2">
+        <v>0.62432900000000002</v>
+      </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1250</v>
       </c>
@@ -7009,8 +7157,32 @@
       <c r="U7">
         <v>0.69409699999999996</v>
       </c>
+      <c r="V7">
+        <v>39133.199999999997</v>
+      </c>
+      <c r="W7">
+        <v>0.62790699999999999</v>
+      </c>
+      <c r="X7">
+        <v>44262.1</v>
+      </c>
+      <c r="Y7">
+        <v>0.63863999999999999</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>31606.5</v>
+      </c>
+      <c r="AA7" s="2">
+        <v>0.58318400000000004</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>53724.1</v>
+      </c>
+      <c r="AC7" s="2">
+        <v>0.62253999999999998</v>
+      </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1500</v>
       </c>
@@ -7074,8 +7246,32 @@
       <c r="U8">
         <v>0.70125199999999999</v>
       </c>
+      <c r="V8">
+        <v>56250.3</v>
+      </c>
+      <c r="W8">
+        <v>0.57960599999999995</v>
+      </c>
+      <c r="X8">
+        <v>66705.899999999994</v>
+      </c>
+      <c r="Y8">
+        <v>0.57781800000000005</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>32380.799999999999</v>
+      </c>
+      <c r="AA8" s="2">
+        <v>0.59928400000000004</v>
+      </c>
+      <c r="AB8" s="2">
+        <v>51800.4</v>
+      </c>
+      <c r="AC8" s="2">
+        <v>0.63685199999999997</v>
+      </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1750</v>
       </c>
@@ -7139,8 +7335,32 @@
       <c r="U9">
         <v>0.70304100000000003</v>
       </c>
+      <c r="V9">
+        <v>57759.4</v>
+      </c>
+      <c r="W9">
+        <v>0.58318400000000004</v>
+      </c>
+      <c r="X9">
+        <v>62047.6</v>
+      </c>
+      <c r="Y9">
+        <v>0.60286200000000001</v>
+      </c>
+      <c r="Z9" s="2">
+        <v>32422.9</v>
+      </c>
+      <c r="AA9" s="2">
+        <v>0.60643999999999998</v>
+      </c>
+      <c r="AB9" s="2">
+        <v>42596.2</v>
+      </c>
+      <c r="AC9" s="2">
+        <v>0.66726300000000005</v>
+      </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2000</v>
       </c>
@@ -7204,8 +7424,32 @@
       <c r="U10">
         <v>0.71556399999999998</v>
       </c>
+      <c r="V10">
+        <v>42688.7</v>
+      </c>
+      <c r="W10">
+        <v>0.617174</v>
+      </c>
+      <c r="X10">
+        <v>48899.6</v>
+      </c>
+      <c r="Y10">
+        <v>0.65652999999999995</v>
+      </c>
+      <c r="Z10" s="2">
+        <v>27498.400000000001</v>
+      </c>
+      <c r="AA10" s="2">
+        <v>0.65295199999999998</v>
+      </c>
+      <c r="AB10" s="2">
+        <v>35039.599999999999</v>
+      </c>
+      <c r="AC10" s="2">
+        <v>0.69767400000000002</v>
+      </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2250</v>
       </c>
@@ -7269,8 +7513,32 @@
       <c r="U11">
         <v>0.72092999999999996</v>
       </c>
+      <c r="V11">
+        <v>34194.400000000001</v>
+      </c>
+      <c r="W11">
+        <v>0.66905199999999998</v>
+      </c>
+      <c r="X11">
+        <v>38527.1</v>
+      </c>
+      <c r="Y11">
+        <v>0.68157400000000001</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>23755.200000000001</v>
+      </c>
+      <c r="AA11" s="2">
+        <v>0.69051899999999999</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>36552.9</v>
+      </c>
+      <c r="AC11" s="2">
+        <v>0.69946299999999995</v>
+      </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2500</v>
       </c>
@@ -7334,8 +7602,32 @@
       <c r="U12">
         <v>0.73345300000000002</v>
       </c>
+      <c r="V12">
+        <v>33242.400000000001</v>
+      </c>
+      <c r="W12">
+        <v>0.67799600000000004</v>
+      </c>
+      <c r="X12">
+        <v>27910.799999999999</v>
+      </c>
+      <c r="Y12">
+        <v>0.738819</v>
+      </c>
+      <c r="Z12" s="2">
+        <v>22804.3</v>
+      </c>
+      <c r="AA12" s="2">
+        <v>0.70304100000000003</v>
+      </c>
+      <c r="AB12" s="2">
+        <v>36017.1</v>
+      </c>
+      <c r="AC12" s="2">
+        <v>0.71019699999999997</v>
+      </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2750</v>
       </c>
@@ -7399,8 +7691,32 @@
       <c r="U13">
         <v>0.73345300000000002</v>
       </c>
+      <c r="V13">
+        <v>34985.699999999997</v>
+      </c>
+      <c r="W13">
+        <v>0.66547400000000001</v>
+      </c>
+      <c r="X13">
+        <v>29869.8</v>
+      </c>
+      <c r="Y13">
+        <v>0.73702999999999996</v>
+      </c>
+      <c r="Z13" s="2">
+        <v>24575.3</v>
+      </c>
+      <c r="AA13" s="2">
+        <v>0.695886</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>43291.6</v>
+      </c>
+      <c r="AC13" s="2">
+        <v>0.68872999999999995</v>
+      </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3000</v>
       </c>
@@ -7464,8 +7780,32 @@
       <c r="U14">
         <v>0.722719</v>
       </c>
+      <c r="V14">
+        <v>38898.300000000003</v>
+      </c>
+      <c r="W14">
+        <v>0.65295199999999998</v>
+      </c>
+      <c r="X14">
+        <v>32091.9</v>
+      </c>
+      <c r="Y14">
+        <v>0.72808600000000001</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>22900</v>
+      </c>
+      <c r="AA14" s="2">
+        <v>0.71556399999999998</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>38764</v>
+      </c>
+      <c r="AC14" s="2">
+        <v>0.70482999999999996</v>
+      </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3250</v>
       </c>
@@ -7529,8 +7869,32 @@
       <c r="U15">
         <v>0.73702999999999996</v>
       </c>
+      <c r="V15">
+        <v>34751.5</v>
+      </c>
+      <c r="W15">
+        <v>0.67799600000000004</v>
+      </c>
+      <c r="X15">
+        <v>34666.5</v>
+      </c>
+      <c r="Y15">
+        <v>0.72629699999999997</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>20001.900000000001</v>
+      </c>
+      <c r="AA15" s="2">
+        <v>0.75670800000000005</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>46375.7</v>
+      </c>
+      <c r="AC15" s="2">
+        <v>0.68515199999999998</v>
+      </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3500</v>
       </c>
@@ -7594,8 +7958,32 @@
       <c r="U16">
         <v>0.74955300000000002</v>
       </c>
+      <c r="V16">
+        <v>32703.4</v>
+      </c>
+      <c r="W16">
+        <v>0.69767400000000002</v>
+      </c>
+      <c r="X16">
+        <v>30937.8</v>
+      </c>
+      <c r="Y16">
+        <v>0.74239699999999997</v>
+      </c>
+      <c r="Z16" s="2">
+        <v>19172.3</v>
+      </c>
+      <c r="AA16" s="2">
+        <v>0.76565300000000003</v>
+      </c>
+      <c r="AB16" s="2">
+        <v>63782.2</v>
+      </c>
+      <c r="AC16" s="2">
+        <v>0.65116300000000005</v>
+      </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3750</v>
       </c>
@@ -7659,8 +8047,32 @@
       <c r="U17">
         <v>0.738819</v>
       </c>
+      <c r="V17">
+        <v>35162.1</v>
+      </c>
+      <c r="W17">
+        <v>0.69230800000000003</v>
+      </c>
+      <c r="X17">
+        <v>35695.9</v>
+      </c>
+      <c r="Y17">
+        <v>0.72987500000000005</v>
+      </c>
+      <c r="Z17" s="2">
+        <v>28155.5</v>
+      </c>
+      <c r="AA17" s="2">
+        <v>0.695886</v>
+      </c>
+      <c r="AB17" s="2">
+        <v>45692.6</v>
+      </c>
+      <c r="AC17" s="2">
+        <v>0.69230800000000003</v>
+      </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>4000</v>
       </c>
@@ -7724,8 +8136,32 @@
       <c r="U18">
         <v>0.73702999999999996</v>
       </c>
+      <c r="V18">
+        <v>36983.1</v>
+      </c>
+      <c r="W18">
+        <v>0.67799600000000004</v>
+      </c>
+      <c r="X18">
+        <v>42445.2</v>
+      </c>
+      <c r="Y18">
+        <v>0.71019699999999997</v>
+      </c>
+      <c r="Z18" s="2">
+        <v>22647.599999999999</v>
+      </c>
+      <c r="AA18" s="2">
+        <v>0.74955300000000002</v>
+      </c>
+      <c r="AB18" s="2">
+        <v>26160.2</v>
+      </c>
+      <c r="AC18" s="2">
+        <v>0.769231</v>
+      </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>4250</v>
       </c>
@@ -7789,8 +8225,32 @@
       <c r="U19">
         <v>0.75313099999999999</v>
       </c>
+      <c r="V19">
+        <v>32100.3</v>
+      </c>
+      <c r="W19">
+        <v>0.706619</v>
+      </c>
+      <c r="X19">
+        <v>39188.5</v>
+      </c>
+      <c r="Y19">
+        <v>0.72808600000000001</v>
+      </c>
+      <c r="Z19" s="2">
+        <v>18977.5</v>
+      </c>
+      <c r="AA19" s="2">
+        <v>0.78712000000000004</v>
+      </c>
+      <c r="AB19" s="2">
+        <v>32126.5</v>
+      </c>
+      <c r="AC19" s="2">
+        <v>0.74418600000000001</v>
+      </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>4500</v>
       </c>
@@ -7854,8 +8314,32 @@
       <c r="U20">
         <v>0.75313099999999999</v>
       </c>
+      <c r="V20">
+        <v>30384.400000000001</v>
+      </c>
+      <c r="W20">
+        <v>0.71735199999999999</v>
+      </c>
+      <c r="X20">
+        <v>34906.800000000003</v>
+      </c>
+      <c r="Y20">
+        <v>0.738819</v>
+      </c>
+      <c r="Z20" s="2">
+        <v>21449</v>
+      </c>
+      <c r="AA20" s="2">
+        <v>0.76565300000000003</v>
+      </c>
+      <c r="AB20" s="2">
+        <v>52127.1</v>
+      </c>
+      <c r="AC20" s="2">
+        <v>0.68694100000000002</v>
+      </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>4750</v>
       </c>
@@ -7919,8 +8403,32 @@
       <c r="U21">
         <v>0.76207499999999995</v>
       </c>
+      <c r="V21">
+        <v>38015.1</v>
+      </c>
+      <c r="W21">
+        <v>0.68515199999999998</v>
+      </c>
+      <c r="X21">
+        <v>32776.6</v>
+      </c>
+      <c r="Y21">
+        <v>0.74239699999999997</v>
+      </c>
+      <c r="Z21" s="2">
+        <v>18981.7</v>
+      </c>
+      <c r="AA21" s="2">
+        <v>0.801431</v>
+      </c>
+      <c r="AB21" s="2">
+        <v>53375</v>
+      </c>
+      <c r="AC21" s="2">
+        <v>0.68872999999999995</v>
+      </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>5000</v>
       </c>
@@ -7984,8 +8492,32 @@
       <c r="U22">
         <v>0.76207499999999995</v>
       </c>
+      <c r="V22">
+        <v>41272.5</v>
+      </c>
+      <c r="W22">
+        <v>0.68872999999999995</v>
+      </c>
+      <c r="X22">
+        <v>30061.1</v>
+      </c>
+      <c r="Y22">
+        <v>0.75491900000000001</v>
+      </c>
+      <c r="Z22" s="2">
+        <v>18419.7</v>
+      </c>
+      <c r="AA22" s="2">
+        <v>0.80858699999999994</v>
+      </c>
+      <c r="AB22" s="2">
+        <v>29476.9</v>
+      </c>
+      <c r="AC22" s="2">
+        <v>0.77638600000000002</v>
+      </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>5250</v>
       </c>
@@ -8049,8 +8581,32 @@
       <c r="U23">
         <v>0.75670800000000005</v>
       </c>
+      <c r="V23">
+        <v>37663.1</v>
+      </c>
+      <c r="W23">
+        <v>0.69409699999999996</v>
+      </c>
+      <c r="X23">
+        <v>29661</v>
+      </c>
+      <c r="Y23">
+        <v>0.75849699999999998</v>
+      </c>
+      <c r="Z23" s="2">
+        <v>20959.599999999999</v>
+      </c>
+      <c r="AA23" s="2">
+        <v>0.78354199999999996</v>
+      </c>
+      <c r="AB23" s="2">
+        <v>28543</v>
+      </c>
+      <c r="AC23" s="2">
+        <v>0.77638600000000002</v>
+      </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>5500</v>
       </c>
@@ -8114,8 +8670,32 @@
       <c r="U24">
         <v>0.77459699999999998</v>
       </c>
+      <c r="V24">
+        <v>29636.2</v>
+      </c>
+      <c r="W24">
+        <v>0.73166399999999998</v>
+      </c>
+      <c r="X24">
+        <v>33858.6</v>
+      </c>
+      <c r="Y24">
+        <v>0.74955300000000002</v>
+      </c>
+      <c r="Z24" s="2">
+        <v>30853.1</v>
+      </c>
+      <c r="AA24" s="2">
+        <v>0.71914100000000003</v>
+      </c>
+      <c r="AB24" s="2">
+        <v>47962.7</v>
+      </c>
+      <c r="AC24" s="2">
+        <v>0.71735199999999999</v>
+      </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>5750</v>
       </c>
@@ -8179,8 +8759,32 @@
       <c r="U25">
         <v>0.78175300000000003</v>
       </c>
+      <c r="V25">
+        <v>26875.599999999999</v>
+      </c>
+      <c r="W25">
+        <v>0.74239699999999997</v>
+      </c>
+      <c r="X25">
+        <v>35452</v>
+      </c>
+      <c r="Y25">
+        <v>0.74597500000000005</v>
+      </c>
+      <c r="Z25" s="2">
+        <v>27298.9</v>
+      </c>
+      <c r="AA25" s="2">
+        <v>0.73524199999999995</v>
+      </c>
+      <c r="AB25" s="2">
+        <v>52745.8</v>
+      </c>
+      <c r="AC25" s="2">
+        <v>0.71019699999999997</v>
+      </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>6000</v>
       </c>
@@ -8244,8 +8848,32 @@
       <c r="U26">
         <v>0.77638600000000002</v>
       </c>
+      <c r="V26">
+        <v>28242</v>
+      </c>
+      <c r="W26">
+        <v>0.738819</v>
+      </c>
+      <c r="X26">
+        <v>31947.4</v>
+      </c>
+      <c r="Y26">
+        <v>0.75670800000000005</v>
+      </c>
+      <c r="Z26" s="2">
+        <v>20612.8</v>
+      </c>
+      <c r="AA26" s="2">
+        <v>0.79606399999999999</v>
+      </c>
+      <c r="AB26" s="2">
+        <v>42826.1</v>
+      </c>
+      <c r="AC26" s="2">
+        <v>0.73524199999999995</v>
+      </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>6250</v>
       </c>
@@ -8309,8 +8937,32 @@
       <c r="U27">
         <v>0.76565300000000003</v>
       </c>
+      <c r="V27">
+        <v>31703.4</v>
+      </c>
+      <c r="W27">
+        <v>0.73166399999999998</v>
+      </c>
+      <c r="X27">
+        <v>27245.7</v>
+      </c>
+      <c r="Y27">
+        <v>0.78175300000000003</v>
+      </c>
+      <c r="Z27" s="2">
+        <v>18472.099999999999</v>
+      </c>
+      <c r="AA27" s="2">
+        <v>0.83363100000000001</v>
+      </c>
+      <c r="AB27" s="2">
+        <v>37249.599999999999</v>
+      </c>
+      <c r="AC27" s="2">
+        <v>0.74776399999999998</v>
+      </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>6500</v>
       </c>
@@ -8374,8 +9026,32 @@
       <c r="U28">
         <v>0.77102000000000004</v>
       </c>
+      <c r="V28">
+        <v>28116.6</v>
+      </c>
+      <c r="W28">
+        <v>0.74239699999999997</v>
+      </c>
+      <c r="X28">
+        <v>22120.9</v>
+      </c>
+      <c r="Y28">
+        <v>0.82289800000000002</v>
+      </c>
+      <c r="Z28" s="2">
+        <v>19445.8</v>
+      </c>
+      <c r="AA28" s="2">
+        <v>0.81753100000000001</v>
+      </c>
+      <c r="AB28" s="2">
+        <v>33543.9</v>
+      </c>
+      <c r="AC28" s="2">
+        <v>0.75491900000000001</v>
+      </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>6750</v>
       </c>
@@ -8439,8 +9115,32 @@
       <c r="U29">
         <v>0.78354199999999996</v>
       </c>
+      <c r="V29">
+        <v>27348.9</v>
+      </c>
+      <c r="W29">
+        <v>0.75491900000000001</v>
+      </c>
+      <c r="X29">
+        <v>22222</v>
+      </c>
+      <c r="Y29">
+        <v>0.82468699999999995</v>
+      </c>
+      <c r="Z29" s="2">
+        <v>30117.8</v>
+      </c>
+      <c r="AA29" s="2">
+        <v>0.72987500000000005</v>
+      </c>
+      <c r="AB29" s="2">
+        <v>32455.5</v>
+      </c>
+      <c r="AC29" s="2">
+        <v>0.75849699999999998</v>
+      </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>7000</v>
       </c>
@@ -8504,8 +9204,32 @@
       <c r="U30">
         <v>0.79427499999999995</v>
       </c>
+      <c r="V30">
+        <v>28982.400000000001</v>
+      </c>
+      <c r="W30">
+        <v>0.74597500000000005</v>
+      </c>
+      <c r="X30">
+        <v>26735.9</v>
+      </c>
+      <c r="Y30">
+        <v>0.79785300000000003</v>
+      </c>
+      <c r="Z30" s="2">
+        <v>27777.1</v>
+      </c>
+      <c r="AA30" s="2">
+        <v>0.74776399999999998</v>
+      </c>
+      <c r="AB30" s="2">
+        <v>37147.9</v>
+      </c>
+      <c r="AC30" s="2">
+        <v>0.74776399999999998</v>
+      </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>7250</v>
       </c>
@@ -8569,8 +9293,32 @@
       <c r="U31">
         <v>0.79069800000000001</v>
       </c>
+      <c r="V31">
+        <v>27904</v>
+      </c>
+      <c r="W31">
+        <v>0.75491900000000001</v>
+      </c>
+      <c r="X31">
+        <v>29123.3</v>
+      </c>
+      <c r="Y31">
+        <v>0.77638600000000002</v>
+      </c>
+      <c r="Z31" s="2">
+        <v>20513.8</v>
+      </c>
+      <c r="AA31" s="2">
+        <v>0.80679800000000002</v>
+      </c>
+      <c r="AB31" s="2">
+        <v>39653.300000000003</v>
+      </c>
+      <c r="AC31" s="2">
+        <v>0.74776399999999998</v>
+      </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>7500</v>
       </c>
@@ -8634,8 +9382,32 @@
       <c r="U32">
         <v>0.79248700000000005</v>
       </c>
+      <c r="V32">
+        <v>24320.3</v>
+      </c>
+      <c r="W32">
+        <v>0.77996399999999999</v>
+      </c>
+      <c r="X32">
+        <v>26865.3</v>
+      </c>
+      <c r="Y32">
+        <v>0.79785300000000003</v>
+      </c>
+      <c r="Z32" s="2">
+        <v>21252.1</v>
+      </c>
+      <c r="AA32" s="2">
+        <v>0.80500899999999997</v>
+      </c>
+      <c r="AB32" s="2">
+        <v>33312.6</v>
+      </c>
+      <c r="AC32" s="2">
+        <v>0.75849699999999998</v>
+      </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>7750</v>
       </c>
@@ -8699,8 +9471,32 @@
       <c r="U33">
         <v>0.75849699999999998</v>
       </c>
+      <c r="V33">
+        <v>23794.5</v>
+      </c>
+      <c r="W33">
+        <v>0.77280899999999997</v>
+      </c>
+      <c r="X33">
+        <v>26480</v>
+      </c>
+      <c r="Y33">
+        <v>0.80679800000000002</v>
+      </c>
+      <c r="Z33" s="2">
+        <v>23848.9</v>
+      </c>
+      <c r="AA33" s="2">
+        <v>0.78175300000000003</v>
+      </c>
+      <c r="AB33" s="2">
+        <v>32005.8</v>
+      </c>
+      <c r="AC33" s="2">
+        <v>0.769231</v>
+      </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>8000</v>
       </c>
@@ -8764,8 +9560,32 @@
       <c r="U34">
         <v>0.77459699999999998</v>
       </c>
+      <c r="V34">
+        <v>23841.599999999999</v>
+      </c>
+      <c r="W34">
+        <v>0.77459699999999998</v>
+      </c>
+      <c r="X34">
+        <v>25701.7</v>
+      </c>
+      <c r="Y34">
+        <v>0.81037599999999999</v>
+      </c>
+      <c r="Z34" s="2">
+        <v>23411.9</v>
+      </c>
+      <c r="AA34" s="2">
+        <v>0.785331</v>
+      </c>
+      <c r="AB34" s="2">
+        <v>36164.300000000003</v>
+      </c>
+      <c r="AC34" s="2">
+        <v>0.75491900000000001</v>
+      </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>8250</v>
       </c>
@@ -8829,8 +9649,32 @@
       <c r="U35">
         <v>0.79606399999999999</v>
       </c>
+      <c r="V35">
+        <v>27778</v>
+      </c>
+      <c r="W35">
+        <v>0.769231</v>
+      </c>
+      <c r="X35">
+        <v>24378.1</v>
+      </c>
+      <c r="Y35">
+        <v>0.81932000000000005</v>
+      </c>
+      <c r="Z35" s="2">
+        <v>22580.3</v>
+      </c>
+      <c r="AA35" s="2">
+        <v>0.801431</v>
+      </c>
+      <c r="AB35" s="2">
+        <v>40671.800000000003</v>
+      </c>
+      <c r="AC35" s="2">
+        <v>0.74955300000000002</v>
+      </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>8500</v>
       </c>
@@ -8894,8 +9738,32 @@
       <c r="U36">
         <v>0.79248700000000005</v>
       </c>
+      <c r="V36">
+        <v>31137.3</v>
+      </c>
+      <c r="W36">
+        <v>0.74418600000000001</v>
+      </c>
+      <c r="X36">
+        <v>25452.6</v>
+      </c>
+      <c r="Y36">
+        <v>0.81753100000000001</v>
+      </c>
+      <c r="Z36" s="2">
+        <v>24233.7</v>
+      </c>
+      <c r="AA36" s="2">
+        <v>0.785331</v>
+      </c>
+      <c r="AB36" s="2">
+        <v>34454.5</v>
+      </c>
+      <c r="AC36" s="2">
+        <v>0.75670800000000005</v>
+      </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>8750</v>
       </c>
@@ -8959,8 +9827,32 @@
       <c r="U37">
         <v>0.80679800000000002</v>
       </c>
+      <c r="V37">
+        <v>24145.200000000001</v>
+      </c>
+      <c r="W37">
+        <v>0.78712000000000004</v>
+      </c>
+      <c r="X37">
+        <v>26503.7</v>
+      </c>
+      <c r="Y37">
+        <v>0.81395300000000004</v>
+      </c>
+      <c r="Z37" s="2">
+        <v>23832.400000000001</v>
+      </c>
+      <c r="AA37" s="2">
+        <v>0.78712000000000004</v>
+      </c>
+      <c r="AB37" s="2">
+        <v>27748.6</v>
+      </c>
+      <c r="AC37" s="2">
+        <v>0.80679800000000002</v>
+      </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>9000</v>
       </c>
@@ -9024,8 +9916,32 @@
       <c r="U38">
         <v>0.80322000000000005</v>
       </c>
+      <c r="V38">
+        <v>23819.599999999999</v>
+      </c>
+      <c r="W38">
+        <v>0.78712000000000004</v>
+      </c>
+      <c r="X38">
+        <v>23835.5</v>
+      </c>
+      <c r="Y38">
+        <v>0.82110899999999998</v>
+      </c>
+      <c r="Z38" s="2">
+        <v>20247</v>
+      </c>
+      <c r="AA38" s="2">
+        <v>0.81753100000000001</v>
+      </c>
+      <c r="AB38" s="2">
+        <v>28895.1</v>
+      </c>
+      <c r="AC38" s="2">
+        <v>0.79964199999999996</v>
+      </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>9250</v>
       </c>
@@ -9089,8 +10005,32 @@
       <c r="U39">
         <v>0.80500899999999997</v>
       </c>
+      <c r="V39">
+        <v>23677.3</v>
+      </c>
+      <c r="W39">
+        <v>0.79964199999999996</v>
+      </c>
+      <c r="X39">
+        <v>27922</v>
+      </c>
+      <c r="Y39">
+        <v>0.80679800000000002</v>
+      </c>
+      <c r="Z39" s="2">
+        <v>20237.5</v>
+      </c>
+      <c r="AA39" s="2">
+        <v>0.82289800000000002</v>
+      </c>
+      <c r="AB39" s="2">
+        <v>31679.9</v>
+      </c>
+      <c r="AC39" s="2">
+        <v>0.77996399999999999</v>
+      </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>9500</v>
       </c>
@@ -9154,8 +10094,32 @@
       <c r="U40">
         <v>0.79964199999999996</v>
       </c>
+      <c r="V40">
+        <v>27654</v>
+      </c>
+      <c r="W40">
+        <v>0.77459699999999998</v>
+      </c>
+      <c r="X40">
+        <v>26055.3</v>
+      </c>
+      <c r="Y40">
+        <v>0.81395300000000004</v>
+      </c>
+      <c r="Z40" s="2">
+        <v>25197.9</v>
+      </c>
+      <c r="AA40" s="2">
+        <v>0.785331</v>
+      </c>
+      <c r="AB40" s="2">
+        <v>38061.1</v>
+      </c>
+      <c r="AC40" s="2">
+        <v>0.75849699999999998</v>
+      </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>9750</v>
       </c>
@@ -9219,8 +10183,32 @@
       <c r="U41">
         <v>0.78354199999999996</v>
       </c>
+      <c r="V41">
+        <v>28308.7</v>
+      </c>
+      <c r="W41">
+        <v>0.77459699999999998</v>
+      </c>
+      <c r="X41">
+        <v>24924.400000000001</v>
+      </c>
+      <c r="Y41">
+        <v>0.81753100000000001</v>
+      </c>
+      <c r="Z41" s="2">
+        <v>25764.5</v>
+      </c>
+      <c r="AA41" s="2">
+        <v>0.78175300000000003</v>
+      </c>
+      <c r="AB41" s="2">
+        <v>36988.800000000003</v>
+      </c>
+      <c r="AC41" s="2">
+        <v>0.75849699999999998</v>
+      </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>10000</v>
       </c>
@@ -9284,8 +10272,32 @@
       <c r="U42">
         <v>0.78890899999999997</v>
       </c>
+      <c r="V42">
+        <v>25291.5</v>
+      </c>
+      <c r="W42">
+        <v>0.78890899999999997</v>
+      </c>
+      <c r="X42">
+        <v>25635.599999999999</v>
+      </c>
+      <c r="Y42">
+        <v>0.81037599999999999</v>
+      </c>
+      <c r="Z42" s="2">
+        <v>25458</v>
+      </c>
+      <c r="AA42" s="2">
+        <v>0.785331</v>
+      </c>
+      <c r="AB42" s="2">
+        <v>32152</v>
+      </c>
+      <c r="AC42" s="2">
+        <v>0.77817499999999995</v>
+      </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B43">
         <f>SUM(B3:B42)</f>
         <v>1807397.6999999993</v>
@@ -9363,11 +10375,43 @@
         <v>1122233.4999999998</v>
       </c>
       <c r="U43" s="3">
-        <f t="shared" ref="D43:U43" si="1">SUM(U3:U42)</f>
+        <f t="shared" ref="D43:W43" si="1">SUM(U3:U42)</f>
         <v>30.023254999999995</v>
       </c>
+      <c r="V43" s="4">
+        <f t="shared" si="1"/>
+        <v>1450051.2000000002</v>
+      </c>
+      <c r="W43" s="3">
+        <f t="shared" si="1"/>
+        <v>28.109121000000002</v>
+      </c>
+      <c r="X43" s="4">
+        <f t="shared" ref="X43" si="2">SUM(X3:X42)</f>
+        <v>1375117.9000000001</v>
+      </c>
+      <c r="Y43" s="3">
+        <f t="shared" ref="Y43" si="3">SUM(Y3:Y42)</f>
+        <v>29.695881000000004</v>
+      </c>
+      <c r="Z43" s="4">
+        <f t="shared" ref="Z43" si="4">SUM(Z3:Z42)</f>
+        <v>1071016.2000000002</v>
+      </c>
+      <c r="AA43" s="3">
+        <f t="shared" ref="AA43" si="5">SUM(AA3:AA42)</f>
+        <v>29.101967999999992</v>
+      </c>
+      <c r="AB43" s="4">
+        <f t="shared" ref="AB43" si="6">SUM(AB3:AB42)</f>
+        <v>1600506.6</v>
+      </c>
+      <c r="AC43" s="3">
+        <f t="shared" ref="AC43" si="7">SUM(AC3:AC42)</f>
+        <v>28.788905999999997</v>
+      </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
     </row>
@@ -11088,51 +12132,54 @@
         <v>26.375674000000004</v>
       </c>
       <c r="D93">
-        <f t="shared" ref="D93:M93" si="2">SUM(D53:D92)</f>
+        <f t="shared" ref="D93:M93" si="8">SUM(D53:D92)</f>
         <v>1155498.8</v>
       </c>
       <c r="E93" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>28.949907999999997</v>
       </c>
       <c r="F93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1415641.4000000004</v>
       </c>
       <c r="G93" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>26.452594000000001</v>
       </c>
       <c r="H93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1299794.9000000001</v>
       </c>
       <c r="I93" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>26.985686999999995</v>
       </c>
       <c r="J93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1060109</v>
       </c>
       <c r="K93" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>29.457963999999993</v>
       </c>
       <c r="L93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1038841.5000000001</v>
       </c>
       <c r="M93" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>30.602861999999998</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="20">
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="B51:C51"/>
     <mergeCell ref="D51:E51"/>

</xml_diff>

<commit_message>
all graphs ready for expore
</commit_message>
<xml_diff>
--- a/lesion_analysis.xlsx
+++ b/lesion_analysis.xlsx
@@ -3653,6 +3653,3085 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>Measuring</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> transferable knowledge in higher layers</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0171650538478874"/>
+          <c:y val="0.0583531214094217"/>
+          <c:w val="0.964517513368071"/>
+          <c:h val="0.859573518457646"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1'!$B$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>blank_eye</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'1'!$A$46:$A$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1750.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2250.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2750.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3250.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3500.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3750.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4250.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4750.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5250.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5500.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5750.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6250.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6500.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6750.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7000.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7250.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7750.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8250.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8500.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8750.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9000.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9250.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9500.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9750.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'1'!$B$46:$B$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.4257605</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4830055</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4812165</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4579605</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.464222</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.47585</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.496422</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.501789</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.50805</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.544723</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.571556</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.588551</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.572451</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.580501</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.592129</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.5912345</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.6189625</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.6359575</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.5992845</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.615385</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.62254</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.649374</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.657424</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.665474</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.678891</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.690519</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.6663685</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.645796</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.659213</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.70483</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.726297</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.7191415</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.6663685</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.686941</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.7057245</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.6547405</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.620751</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.644007</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.68873</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.7227195</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1'!$C$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>wallet_eye</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'1'!$A$46:$A$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1750.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2250.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2750.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3250.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3500.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3750.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4250.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4750.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5250.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5500.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5750.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6250.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6500.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6750.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7000.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7250.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7750.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8250.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8500.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8750.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9000.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9250.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9500.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9750.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'1'!$C$46:$C$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.7155635</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.635957</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.625224</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.677996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7003575</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6887295</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.673524</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.728086</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7513415</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.736136</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.6958855</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.7173525</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.757603</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.767442</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.7567085</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.736136</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.734347</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.754025</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.773703</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.748658</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.773703</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.7719145</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.77907</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.7665475</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.7629695</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.7432915</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.7504475</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.775492</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.7942755</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.805009</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.7960645</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.779964</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.7772805</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.7960645</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.8067975</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.8059035</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.808587</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.800537</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.7978535</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.78712</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1'!$D$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>wallet_eye_000111</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'1'!$A$46:$A$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1750.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2250.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2750.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3250.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3500.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3750.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4250.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4750.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5250.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5500.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5750.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6250.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6500.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6750.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7000.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7250.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7750.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8250.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8500.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8750.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9000.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9250.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9500.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9750.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'1'!$D$46:$D$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.577818</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.60644</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.631485</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.649374</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.658318</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.676208</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.694097</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.692308</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.713775</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.706619</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.690519</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.710197</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.713775</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.722719</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.728086</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.728086</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.742397</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.762075</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.77102</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.77102</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.751342</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.769231</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.778175</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.781753</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.767442</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.765653</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.78712</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.785331</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.785331</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.779964</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.783542</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.783542</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.78712</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.792487</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.788909</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.785331</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.788909</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.785331</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.788909</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.797853</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1'!$E$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>wallet_eye_111000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'1'!$A$46:$A$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1750.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2250.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2750.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3250.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3500.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3750.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4250.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4750.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5250.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5500.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5750.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6250.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6500.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6750.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7000.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7250.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7750.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8250.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8500.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8750.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9000.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9250.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9500.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9750.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'1'!$E$46:$E$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.515206</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.45975</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.457961</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.47585</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.497317</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.502683</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.511628</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.52415</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.538462</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.563506</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.57424</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.568873</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.556351</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.604651</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.611807</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.613596</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.62254</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.624329</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.627907</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.620751</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.645796</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.670841</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.676208</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.683363</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.699463</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.68873</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.70483</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.713775</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.717352</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.67263</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.676208</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.711986</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.735242</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.735242</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.744186</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.747764</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.749553</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.747764</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.751342</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.754919</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1'!$F$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>wallet_eye_111001</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'1'!$A$46:$A$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1750.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2250.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2750.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3250.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3500.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3750.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4250.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4750.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5250.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5500.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5750.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6250.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6500.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6750.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7000.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7250.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7750.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8250.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8500.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8750.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9000.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9250.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9500.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9750.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'1'!$F$46:$F$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.547406</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.520572</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.533095</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.592129</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.635063</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.663685</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.660107</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.651163</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.692308</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.710197</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.710197</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.710197</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.722719</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.753131</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.77102</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.767442</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.710197</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.706619</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.763864</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.769231</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.774597</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.767442</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.765653</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.77102</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.78712</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.788909</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.754919</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.742397</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.785331</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.785331</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.805009</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.783542</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.78712</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.808587</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.801431</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.794275</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.808587</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.808587</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.817531</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.815742</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1'!$G$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>wallet_eye_110000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'1'!$A$46:$A$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1750.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2250.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2750.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3250.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3500.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3750.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4250.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4750.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5250.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5500.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5750.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6250.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6500.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6750.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7000.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7250.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7750.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8250.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8500.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8750.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9000.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9250.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9500.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9750.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'1'!$G$46:$G$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.468694</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.472272</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.525939</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.484794</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.499106</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.516995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.559928</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.584973</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.584973</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.556351</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.601073</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.640429</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.651163</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.642218</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.611807</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.608229</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.654741</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.68873</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.685152</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.677996</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.679785</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.697674</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.713775</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.697674</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.699463</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.701252</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.706619</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.699463</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.692308</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.706619</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.713775</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.710197</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.710197</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.713775</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.715564</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.717352</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.722719</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.735242</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.747764</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.763864</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1'!$H$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>wallet_eye_100000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'1'!$A$46:$A$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1750.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2250.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2750.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3250.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3500.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3750.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4250.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4750.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5250.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5500.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5750.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6250.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6500.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6750.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7000.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7250.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7750.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8250.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8500.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8750.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9000.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9250.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9500.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9750.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'1'!$H$46:$H$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.611807</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.629696</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6610015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6529515</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6583185</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.669052</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.685152</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.706619</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7101965</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.721825</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7110915</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.7137745</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.711091</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.700358</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.7155635</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.7531305</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.7486585</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.720036</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.7254025</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.7692305</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.766547</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.7459745</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.745975</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.755814</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.7567085</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.7629695</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.7710195</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.7710195</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.769231</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.775492</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.763864</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.764758</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.7728085</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.7745975</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.806798</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.801431</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.7924865</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.7790695</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.7710195</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.783542</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1'!$I$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>wallet_eye_100001</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'1'!$A$46:$A$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1750.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2250.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2750.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3250.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3500.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3750.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4250.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4750.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5250.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5500.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5750.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6250.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6500.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6750.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7000.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7250.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7750.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8250.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8500.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8750.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9000.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9250.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9500.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9750.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'1'!$I$46:$I$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.4758495</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.570662</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5822895</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6350625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.610912</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.588551</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.604651</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.654741</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.6860465</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.72093</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.716458</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.721825</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.7415025</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.754025</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.7128805</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.729875</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.757603</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.752236</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.771914</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.781753</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.7710195</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.734347</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.7406085</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.776386</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.807692</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.8202145</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.777281</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.7728085</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.791592</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.801431</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.7942755</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.7978535</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.8103755</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.801431</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.8005365</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.81932</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.814848</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.799642</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.799642</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.7978535</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1'!$J$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>wallet_eye_000001</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'1'!$A$46:$A$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1750.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2250.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2750.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3250.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3500.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3750.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4250.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4750.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5250.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5500.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5750.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6250.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6500.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6750.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7000.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7250.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7750.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8250.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8500.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8750.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9000.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9250.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9500.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9750.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'1'!$J$46:$J$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.325581</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.370304</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.386404</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.481216</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.533095</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.518784</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.522361</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.527728</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.593918</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.667263</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.683363</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.683363</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.683363</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.708408</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.726297</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.733453</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.697674</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.697674</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.744186</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.763864</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.77102</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.767442</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.769231</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.778175</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.774597</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.788909</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.794275</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.781753</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.785331</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.790698</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.80322</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.80322</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.812165</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.808587</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.810376</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.821109</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.828265</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.831843</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.833631</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.833631</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1998574240"/>
+        <c:axId val="1826810528"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1998574240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10000.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1826810528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1826810528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.3"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1998574240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="4"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="5"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="6"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="7"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="8"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="11"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>Test Accuracy</a:t>
             </a:r>
           </a:p>
@@ -6379,7 +9458,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -8710,6 +11789,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -10285,6 +13404,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -10835,15 +14470,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>253999</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>73025</xdr:rowOff>
+      <xdr:colOff>809624</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>136525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>396874</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>126999</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10857,6 +14492,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>111125</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -11195,8 +14862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K51" workbookViewId="0">
-      <selection activeCell="U87" sqref="U87"/>
+    <sheetView tabSelected="1" topLeftCell="K62" workbookViewId="0">
+      <selection activeCell="W90" sqref="W90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>